<commit_message>
saves copy of second most recent spreadsheets for reference
</commit_message>
<xml_diff>
--- a/xls/old/CeramicVessels.xlsx
+++ b/xls/old/CeramicVessels.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Salmon Whole Pots'!$A$1:$R$332</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -3146,7 +3146,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="62.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>